<commit_message>
Playoffs bones set up. I messed something up in play_ball, not sure why it can't resolve team1 and team2 anymore. Didn't think my moving of stuff out of the main method would have caused it
</commit_message>
<xml_diff>
--- a/Data/Playoff Rosters Reformatted.xlsx
+++ b/Data/Playoff Rosters Reformatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\321bm\Documents\George Mason\Courses\OR 635\Project\OR635-Baseball-Simulation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CF3095-BF8A-48E4-8763-51AA0B395DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DEB557-C111-428F-B908-29CE6E4810E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6D96AF30-26F2-49DA-96ED-7E60884DD9EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="12" xr2:uid="{6D96AF30-26F2-49DA-96ED-7E60884DD9EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -1497,7 +1497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB66AE08-7414-42B7-B43D-819C9726F006}">
   <dimension ref="A2:AV31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+    <sheetView topLeftCell="AK1" workbookViewId="0">
       <selection activeCell="AU20" sqref="AU20"/>
     </sheetView>
   </sheetViews>
@@ -5045,7 +5045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D71278-6547-4CCB-8DF2-A360901A7C72}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>